<commit_message>
MNO template spreadsheet: update with latest list of networks
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benilovj/workspace/dfe/get-help-with-tech/public/collecting-mobile-information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82E7E5E-26B8-C540-8176-CF302A967C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DWk/iI7WJL6C+29bLNvgmP9ozehQ9C9oeiDq1CRor61tRCfOkNhTAafC0gPhAS1sBd0CH8+wSoDIet5MQgj1pA==" workbookSaltValue="hAOPV+djOyk2S2VTK2Zbvw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B74C7A-547F-6544-B102-53CF6C50F9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DiRHWy9HBtWSiUHjm+6iZ9h2C25vMf09dfPtZGPMJ6pd/MR7+womHx+HYhT1574Dw9gixmt/yD0RVtnnFJi+Tw==" workbookSaltValue="AESE6F2eULHdKZDcbfVhWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Account holder name</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>EE</t>
-  </si>
-  <si>
-    <t>O2</t>
   </si>
   <si>
     <t>Sky Mobile</t>
@@ -167,8 +164,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A8" totalsRowShown="0">
-  <autoFilter ref="A1:A8" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A7" totalsRowShown="0">
+  <autoFilter ref="A1:A7" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68819AC5-C385-E146-A96D-0402A116A9B3}" name="Mobile networks"/>
   </tableColumns>
@@ -496,7 +493,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -528,16 +525,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>1</v>
@@ -554,12 +551,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00F40AAC-2AA1-3749-A21F-0DE2096DC427}">
-          <x14:formula1>
-            <xm:f>'Mobile networks'!$A$2:$A$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5017466D-08F8-824E-8483-82E2A844911E}">
           <x14:formula1>
             <xm:f>'Subscriber type'!$A$2:$A$3</xm:f>
@@ -572,6 +563,12 @@
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00F40AAC-2AA1-3749-A21F-0DE2096DC427}">
+          <x14:formula1>
+            <xm:f>'Mobile networks'!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -580,10 +577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D2E559-5640-1345-A414-9CCC724082EB}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,7 +590,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -626,13 +623,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MJyj8+5k3I/oylNt6vpYtyvCuNoPImFgSbr8H0JiSj5DTGDtc8a4E1cLegFlxVF4PTD9mz0Hr2eF6YyPH9VOgw==" saltValue="ZZ5IvGwucc4izKW4g6NSuw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qYwvrt+sKR4MwdW7PqYAe4svJrT3fY7kN3ZoWNSsJ1Raqs4ST8kk7ICLWvL0IBT1ExpnkM6yW4fkGoP2ktb0Dg==" saltValue="gRxlKqW/YCwfKATT79yUrg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -655,17 +647,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +682,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Vodafone to participating mnos but remove any user accesss
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benilovj/workspace/dfe/get-help-with-tech/public/collecting-mobile-information/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B74C7A-547F-6544-B102-53CF6C50F9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DiRHWy9HBtWSiUHjm+6iZ9h2C25vMf09dfPtZGPMJ6pd/MR7+womHx+HYhT1574Dw9gixmt/yD0RVtnnFJi+Tw==" workbookSaltValue="AESE6F2eULHdKZDcbfVhWw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67A7A31-45A3-2247-A5F2-4EA970B0D417}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="tr/7KuuLMf7W8bNme74/d/5wTB+mHQGA1xDaepZG8idGM+ddXUSOeHwYBXs+/6cR4kSWky2PQOvI2UsC67+VEQ==" workbookSaltValue="cEiGR9HVNpymPKrSOzn5gA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
+    <workbookView xWindow="1340" yWindow="680" windowWidth="32580" windowHeight="19460" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Extra mobile data requests" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Account holder name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Pay monthly or PAYG?</t>
+  </si>
+  <si>
+    <t>Vodafone</t>
   </si>
 </sst>
 </file>
@@ -164,8 +167,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A7" totalsRowShown="0">
-  <autoFilter ref="A1:A7" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A8" totalsRowShown="0">
+  <autoFilter ref="A1:A8" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68819AC5-C385-E146-A96D-0402A116A9B3}" name="Mobile networks"/>
   </tableColumns>
@@ -541,7 +544,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KtFFbYXrVF54CgJuMbuDxaVkhxF9KmBcOwawQdCeCkaDQmM1LrsZS7QcjDN2TmVgkK4+wbdYALp8kzSBh0f3bQ==" saltValue="k+QOqRKton2eRp5kdgBTYQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="H79p17KsuvfCX4QbIYNARFibJFgETMoGyDanHfKLlOQXtcZFUb6kqiztXhoaa7hYjgiuzMtJ3D848S7pXaRP4Q==" saltValue="sh1IxqxMyWCbM/PA3Srshg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{627EC1B1-E4D4-C747-B692-2D3AFD8AE7AB}">
       <formula1>EXACT(LEFT(B2, 2), "07")</formula1>
@@ -565,7 +568,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00F40AAC-2AA1-3749-A21F-0DE2096DC427}">
           <x14:formula1>
-            <xm:f>'Mobile networks'!$A$2:$A$7</xm:f>
+            <xm:f>'Mobile networks'!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -577,10 +580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D2E559-5640-1345-A414-9CCC724082EB}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,8 +626,13 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qYwvrt+sKR4MwdW7PqYAe4svJrT3fY7kN3ZoWNSsJ1Raqs4ST8kk7ICLWvL0IBT1ExpnkM6yW4fkGoP2ktb0Dg==" saltValue="gRxlKqW/YCwfKATT79yUrg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rDMmQSg9mgm8igW+gEYeJxM/aQj/e24/+cvhSTbM5rbXkm8VT9xq0Y4qsMO1uycXtt9Ixjlq8JaZCtcsVdrUzg==" saltValue="0CamvZ1k8PGz8Weo5EZ+Gw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Added O2 to mno bulk request spreadsheet
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Work/dfe/get-help-with-tech/public/collecting-mobile-information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67A7A31-45A3-2247-A5F2-4EA970B0D417}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="tr/7KuuLMf7W8bNme74/d/5wTB+mHQGA1xDaepZG8idGM+ddXUSOeHwYBXs+/6cR4kSWky2PQOvI2UsC67+VEQ==" workbookSaltValue="cEiGR9HVNpymPKrSOzn5gA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794DF5EE-FA51-8C44-A44D-AADE4429F7A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="plyY9D8eWqDCqpF82SeuCDRis4LfhGxZwm1v8f1+stVPN8Qomclj3VkO1TJwJkPGGl+hl3198wpvCFO0B8pvUA==" workbookSaltValue="LlV9t6aFY8iewSCU89Du1g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="680" windowWidth="32580" windowHeight="19460" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Account holder name</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Vodafone</t>
+  </si>
+  <si>
+    <t>O2</t>
   </si>
 </sst>
 </file>
@@ -167,8 +170,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A8" totalsRowShown="0">
-  <autoFilter ref="A1:A8" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A9" totalsRowShown="0">
+  <autoFilter ref="A1:A9" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68819AC5-C385-E146-A96D-0402A116A9B3}" name="Mobile networks"/>
   </tableColumns>
@@ -568,7 +571,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00F40AAC-2AA1-3749-A21F-0DE2096DC427}">
           <x14:formula1>
-            <xm:f>'Mobile networks'!$A$2:$A$8</xm:f>
+            <xm:f>'Mobile networks'!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D2E559-5640-1345-A414-9CCC724082EB}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,36 +606,41 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rDMmQSg9mgm8igW+gEYeJxM/aQj/e24/+cvhSTbM5rbXkm8VT9xq0Y4qsMO1uycXtt9Ixjlq8JaZCtcsVdrUzg==" saltValue="0CamvZ1k8PGz8Weo5EZ+Gw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="BVAvRQcP/0vUBzA5Ohv8QKtjqfn4eqjy7jya9GBhKdf4YrV2JmkaJ3Y8a/C3gp9ayvOz6kJ/w8Wc/vIKuoNn+g==" saltValue="2MDsb86PcUShHgisMZtgMw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Added BT Mobile and Lycamobile to the spreadsheet template
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Work/dfe/get-help-with-tech/public/collecting-mobile-information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794DF5EE-FA51-8C44-A44D-AADE4429F7A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="plyY9D8eWqDCqpF82SeuCDRis4LfhGxZwm1v8f1+stVPN8Qomclj3VkO1TJwJkPGGl+hl3198wpvCFO0B8pvUA==" workbookSaltValue="LlV9t6aFY8iewSCU89Du1g==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5419EC-DE7B-8A4C-A39F-128D3B60FE56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QxNmE7Gb6Qg5D1JnTtQPKXS+kFF+0c/Knxjz9odQJG36HwcTr0T1ClWF1MDSReXWTeOEVxTmNmDE5lP8s1yV2w==" workbookSaltValue="k49Z0RDfSltxRySG1gPnGA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="680" windowWidth="32580" windowHeight="19460" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Account holder name</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>O2</t>
+  </si>
+  <si>
+    <t>BT Mobile</t>
+  </si>
+  <si>
+    <t>Lycamobile</t>
   </si>
 </sst>
 </file>
@@ -170,8 +176,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A9" totalsRowShown="0">
-  <autoFilter ref="A1:A9" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9564E200-739F-E247-86FA-F8779A49393D}" name="Table3" displayName="Table3" ref="A1:A11" totalsRowShown="0">
+  <autoFilter ref="A1:A11" xr:uid="{F9017BE4-5038-B044-A887-7F3304ACCDAD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68819AC5-C385-E146-A96D-0402A116A9B3}" name="Mobile networks"/>
   </tableColumns>
@@ -537,10 +543,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>1</v>
@@ -571,7 +577,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00F40AAC-2AA1-3749-A21F-0DE2096DC427}">
           <x14:formula1>
-            <xm:f>'Mobile networks'!$A$2:$A$9</xm:f>
+            <xm:f>'Mobile networks'!$A$2:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -583,10 +589,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D2E559-5640-1345-A414-9CCC724082EB}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,46 +607,56 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="BVAvRQcP/0vUBzA5Ohv8QKtjqfn4eqjy7jya9GBhKdf4YrV2JmkaJ3Y8a/C3gp9ayvOz6kJ/w8Wc/vIKuoNn+g==" saltValue="2MDsb86PcUShHgisMZtgMw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XYVFsbn6A9rSTB8d2SCfRsSjF1ydraHcbO2GbpcpQHgwEGQtRYQl9jT6L2CmOyaSKeE0KgYVqIzA6YJBo6qh8g==" saltValue="pFgeBqcZdH69uzLV36vNEw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
add IQ Mobile as a participating MobileNetwork
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -236,7 +236,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -341,7 +341,7 @@
       <c r="E10" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D10" type="list">
       <formula1>"Pay monthly,Pay-as-you-go (PAYG)"</formula1>
       <formula2>0</formula2>
@@ -350,12 +350,8 @@
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C10" type="list">
-      <formula1>",BT Mobile,EE,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2" type="list">
-      <formula1>"BT Mobile,EE,giffgaff,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C10" type="list">
+      <formula1>"BT Mobile,EE,giffgaff,iQ Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -377,7 +373,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C2:C10 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,7 +518,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,7 +622,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[1716] add IQ Mobile as a participating MobileNetwork (#1440)
* add IQ Mobile as a participating MobileNetwork

* rubocop fix
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -236,7 +236,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -341,7 +341,7 @@
       <c r="E10" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D10" type="list">
       <formula1>"Pay monthly,Pay-as-you-go (PAYG)"</formula1>
       <formula2>0</formula2>
@@ -350,12 +350,8 @@
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C10" type="list">
-      <formula1>",BT Mobile,EE,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2" type="list">
-      <formula1>"BT Mobile,EE,giffgaff,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C10" type="list">
+      <formula1>"BT Mobile,EE,giffgaff,iQ Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -377,7 +373,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C2:C10 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,7 +518,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,7 +622,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add Asda Mobile to xlsx validation list after rebase
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -233,10 +233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C10"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -340,6 +340,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
     </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D10" type="list">
@@ -351,7 +352,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C10" type="list">
-      <formula1>"BT Mobile,EE,giffgaff,iQ Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
+      <formula1>"Asda Mobile,BT Mobile,EE,giffgaff,iQ Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -373,7 +374,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C2:C10 B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -518,7 +519,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,7 +623,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
make sure Lebara Mobile are also in the spreadsheet
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -236,7 +236,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,7 +352,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C10" type="list">
-      <formula1>"Asda Mobile,BT Mobile,EE,giffgaff,iQ Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
+      <formula1>"Asda Mobile,BT Mobile,EE,giffgaff,iQ Mobile,Lebara Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
1717 add Asda Mobile as a participating mobile network (#1426)
* add asda mobile to the service

* add migration

* remove PAYG hyphens as per @LloydK

* add Asda Mobile to xlsx validation list after rebase

* make sure Lebara Mobile are also in the spreadsheet
</commit_message>
<xml_diff>
--- a/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
+++ b/public/collecting-mobile-information/extra-mobile-data-requests-template.xlsx
@@ -233,10 +233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C10"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -340,6 +340,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
     </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D10" type="list">
@@ -351,7 +352,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C10" type="list">
-      <formula1>"BT Mobile,EE,giffgaff,iQ Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
+      <formula1>"Asda Mobile,BT Mobile,EE,giffgaff,iQ Mobile,Lebara Mobile,Lycamobile,O2,Sky Mobile,SMARTY,Tesco Mobile,Three,Virgin Mobile,Vodafone,iD Mobile"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -373,7 +374,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C2:C10 B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -518,7 +519,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,7 +623,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>